<commit_message>
login page test chnged
</commit_message>
<xml_diff>
--- a/src/main/java/com/Testdata/Data_asign.xlsx
+++ b/src/main/java/com/Testdata/Data_asign.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15465" windowHeight="5580" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13440" windowHeight="5580" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,15 +12,14 @@
     <sheet name="NewtourRegister" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
     <sheet name="OHRMaddE" sheetId="6" r:id="rId5"/>
-    <sheet name="emp" r:id="rId9" sheetId="7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O17"/>
+  <oleSize ref="A1:M17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>mahesh</t>
   </si>
@@ -182,61 +181,12 @@
   </si>
   <si>
     <t>nani</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>0003</t>
-  </si>
-  <si>
-    <t>0008</t>
-  </si>
-  <si>
-    <t>0013</t>
-  </si>
-  <si>
-    <t>0001</t>
-  </si>
-  <si>
-    <t>0006</t>
-  </si>
-  <si>
-    <t>0011</t>
-  </si>
-  <si>
-    <t>0002</t>
-  </si>
-  <si>
-    <t>0007</t>
-  </si>
-  <si>
-    <t>0012</t>
-  </si>
-  <si>
-    <t>0004</t>
-  </si>
-  <si>
-    <t>0009</t>
-  </si>
-  <si>
-    <t>0014</t>
-  </si>
-  <si>
-    <t>0005</t>
-  </si>
-  <si>
-    <t>0010</t>
-  </si>
-  <si>
-    <t>0015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -626,9 +576,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -690,9 +640,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -745,8 +695,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -796,8 +746,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -914,13 +864,13 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -974,407 +924,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>